<commit_message>
feat: Add kelas field to User and Candidates models
This commit adds the `kelas` field to the `User` and `Candidates` models in the database schema. It also includes the necessary database migrations and updates the corresponding components to handle the new field.
</commit_message>
<xml_diff>
--- a/public/template-excel/users.xlsx
+++ b/public/template-excel/users.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/dev/pilketos-moklet/public/template-excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMK TELKOM 003\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B50DFA-B96A-0341-9741-86BED8DDB8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB815C4-8C25-42AA-B9B5-037DB17ECA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{DF77CB2D-1FC9-7A4D-A8EB-AA246A23A53C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DF77CB2D-1FC9-7A4D-A8EB-AA246A23A53C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="xr1" sheetId="1" r:id="rId1"/>
+    <sheet name="xr2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -143,8 +143,117 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Kusindra Aji Rabbany</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CA8138D6-AAFA-42CA-95D4-F9CB6D2D67A7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kusindra Aji Rabbany:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If the email already exists in the database, it will be updated according to the data in excel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{7C4D9A02-BD70-46F1-9C42-18C2113B0753}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kusindra Aji Rabbany:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>If not filled in, the role will be set based on email. If there is .student, it will get the role student, otherwise it will get the role teacher</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{6ADC83C9-53E4-4C11-B602-F7C299C12F87}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kusindra Aji Rabbany:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Password is optional. If not filled, will be generated by the system</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Email</t>
   </si>
@@ -152,16 +261,22 @@
     <t>Name</t>
   </si>
   <si>
-    <t>kusindra_rabbany_31rpl@student.smktelkom-mlg.sch.id</t>
-  </si>
-  <si>
-    <t>Kusindra Aji Rabbany 31 RPL</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>naufal_nabil_32rpl@student.smktelkom-mlg.sch.id</t>
+  </si>
+  <si>
+    <t>Naufal Nabil Ramadhan 32 RPL</t>
+  </si>
+  <si>
+    <t>Kelas</t>
+  </si>
+  <si>
+    <t>XI RPL 6</t>
   </si>
 </sst>
 </file>
@@ -539,18 +654,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143AC0F7-DD21-6B40-89B5-EDEE3F112EBD}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="50.5" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.296875" customWidth="1"/>
+    <col min="3" max="3" width="22.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -558,18 +673,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -579,4 +694,57 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1F12C2-5554-4C3D-B5F2-8ECC57CC0CC7}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.796875" customWidth="1"/>
+    <col min="2" max="3" width="30.59765625" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="33.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F7C5ECDC-9782-4146-8944-76E6622DE2D0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add vote session access dashboard
</commit_message>
<xml_diff>
--- a/public/template-excel/users.xlsx
+++ b/public/template-excel/users.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMK TELKOM 003\OneDrive\Documents\Folder Programing Website\e-pilketos\public\template-excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/dev/e-pilketos-moklet/public/template-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEB43C8-2085-4ED2-BCD1-CBCB137AEA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5290FF43-9C4A-F644-BC8A-7DF2C71D0726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DF77CB2D-1FC9-7A4D-A8EB-AA246A23A53C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="12460" xr2:uid="{DF77CB2D-1FC9-7A4D-A8EB-AA246A23A53C}"/>
   </bookViews>
   <sheets>
-    <sheet name="xr1" sheetId="1" r:id="rId1"/>
-    <sheet name="xr2" sheetId="2" r:id="rId2"/>
+    <sheet name="Users" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -139,17 +138,7 @@
         </r>
       </text>
     </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Kusindra Aji Rabbany</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CA8138D6-AAFA-42CA-95D4-F9CB6D2D67A7}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{E1591034-78F6-5947-83CD-0FB1C95BF8AF}">
       <text>
         <r>
           <rPr>
@@ -178,73 +167,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>If the email already exists in the database, it will be updated according to the data in excel.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{7C4D9A02-BD70-46F1-9C42-18C2113B0753}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Kusindra Aji Rabbany:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>If not filled in, the role will be set based on email. If there is .student, it will get the role student, otherwise it will get the role teacher</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{6ADC83C9-53E4-4C11-B602-F7C299C12F87}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Kusindra Aji Rabbany:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Password is optional. If not filled, will be generated by the system</t>
+          <t>Optional</t>
         </r>
       </text>
     </comment>
@@ -253,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Email</t>
   </si>
@@ -267,10 +190,13 @@
     <t>Password</t>
   </si>
   <si>
-    <t>naufal_nabil_32rpl@student.smktelkom-mlg.sch.id</t>
+    <t>Kelas</t>
   </si>
   <si>
-    <t>Naufal Nabil Ramadhan 32 RPL</t>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -646,20 +572,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143AC0F7-DD21-6B40-89B5-EDEE3F112EBD}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.5" customWidth="1"/>
-    <col min="2" max="2" width="24.296875" customWidth="1"/>
-    <col min="3" max="3" width="22.19921875" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,65 +598,21 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{A10CDF8A-C7BF-DB4B-992D-7A232000849E}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1F12C2-5554-4C3D-B5F2-8ECC57CC0CC7}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="42.796875" customWidth="1"/>
-    <col min="2" max="2" width="30.59765625" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="33.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{F7C5ECDC-9782-4146-8944-76E6622DE2D0}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{DD62F04D-F054-D942-B50A-5AB8E7DCC999}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>